<commit_message>
benchmark intarna, risearch2, riblast
</commit_message>
<xml_diff>
--- a/benchmark/benchmark-data.xlsx
+++ b/benchmark/benchmark-data.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qubsq01\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Research\Artikel\CheRRI\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C76A8F-2E63-49C4-8947-7AAA541D161F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21970A31-15B2-425C-BE71-9E9CD8FE9DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="-120" windowWidth="37050" windowHeight="21840" xr2:uid="{A8F6821C-00DF-431A-B3FF-F884BE8DA56B}"/>
+    <workbookView xWindow="1590" yWindow="0" windowWidth="18405" windowHeight="21600" xr2:uid="{A8F6821C-00DF-431A-B3FF-F884BE8DA56B}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="benchmark-data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="280">
   <si>
     <t>ug.1</t>
   </si>
@@ -407,9 +407,6 @@
     <t>ACA35</t>
   </si>
   <si>
-    <t>U2 snRNA</t>
-  </si>
-  <si>
     <t>H/ACA snoRNA (scaRNA)</t>
   </si>
   <si>
@@ -816,13 +813,76 @@
   </si>
   <si>
     <t>organism</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>RNU6-1</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>not annotated</t>
+  </si>
+  <si>
+    <t>exons</t>
+  </si>
+  <si>
+    <t>mismatches!</t>
+  </si>
+  <si>
+    <t>mir101-1</t>
+  </si>
+  <si>
+    <t>mir24-1</t>
+  </si>
+  <si>
+    <t>mir26a1</t>
+  </si>
+  <si>
+    <t>mir29b1</t>
+  </si>
+  <si>
+    <t>mirlet7a1</t>
+  </si>
+  <si>
+    <t>qHg38Start</t>
+  </si>
+  <si>
+    <t>qHg38Strand</t>
+  </si>
+  <si>
+    <t>qHg38Chr</t>
+  </si>
+  <si>
+    <t>qHg38Notes</t>
+  </si>
+  <si>
+    <t>Zz</t>
+  </si>
+  <si>
+    <t>tHg38Chr</t>
+  </si>
+  <si>
+    <t>tHg38Strand</t>
+  </si>
+  <si>
+    <t>tHg38Start</t>
+  </si>
+  <si>
+    <t>tHg38Notes</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -855,13 +915,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -878,25 +949,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -1213,18 +1285,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245A010E-8F99-4A7A-AC12-56117D06DCFC}">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="P50" sqref="P50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="8" max="9" width="11.42578125" style="6"/>
+    <col min="15" max="16" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1238,1392 +1312,2166 @@
         <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F1" t="s">
         <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>256</v>
-      </c>
-      <c r="H1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="J1" t="s">
+        <v>270</v>
+      </c>
+      <c r="K1" t="s">
+        <v>273</v>
+      </c>
+      <c r="L1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
+        <v>257</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>277</v>
+      </c>
+      <c r="R1" t="s">
+        <v>278</v>
+      </c>
+      <c r="S1" t="s">
         <v>258</v>
       </c>
-      <c r="J1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="6">
+        <v>2</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J2" s="3">
+        <v>231456444</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="M2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="N2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="O2" s="6">
+        <v>21</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>8392666</v>
+      </c>
+      <c r="R2" t="s">
+        <v>262</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="6">
+        <v>22</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J3" s="3">
+        <v>39319052</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="M3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="N3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="O3" s="6">
+        <v>21</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>8392666</v>
+      </c>
+      <c r="R3" t="s">
+        <v>262</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="6">
+        <v>16</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J4" s="3">
+        <v>71758402</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="M4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="N4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="O4" s="6">
+        <v>21</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>8256780</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="6">
+        <v>5</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J5" s="3">
+        <v>181241818</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="M5" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="N5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="O5" s="6">
+        <v>21</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>8256780</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="F6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="6">
+        <v>11</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J6" s="3">
+        <v>62855012</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="M6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="N6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="O6" s="6">
+        <v>21</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>8392666</v>
+      </c>
+      <c r="R6" t="s">
+        <v>262</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="F7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="6">
+        <v>15</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J7" s="3">
+        <v>66502811</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="M7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="N7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="O7" s="6">
+        <v>21</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>8392666</v>
+      </c>
+      <c r="R7" t="s">
+        <v>262</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="6">
+        <v>2</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J8" s="3">
+        <v>206161881</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="M8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="N8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="O8" s="6">
+        <v>21</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>8441146</v>
+      </c>
+      <c r="R8" t="s">
+        <v>262</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="6">
+        <v>8</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J9" s="3">
+        <v>98042086</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="M9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="N9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K9" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="O9" s="6">
+        <v>21</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>8256780</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="F10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J10" s="3">
+        <v>119787353</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="M10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="N10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K10" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="O10" s="6">
+        <v>21</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>8256780</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="F11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="6">
+        <v>17</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J11" s="3">
+        <v>7577955</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="M11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="N11" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="O11" s="6">
+        <v>21</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>8392666</v>
+      </c>
+      <c r="R11" t="s">
+        <v>262</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="F12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="6">
+        <v>2</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J12" s="3">
+        <v>231455800</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="M12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="N12" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="K12" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="O12" s="6">
+        <v>21</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>8392666</v>
+      </c>
+      <c r="R12" t="s">
+        <v>262</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="F13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="6">
+        <v>11</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="J13" s="3">
+        <v>93735110</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="M13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="N13" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K13" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="O13" s="6">
+        <v>21</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>8392666</v>
+      </c>
+      <c r="R13" t="s">
+        <v>262</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="C14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="F14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="6">
+        <v>11</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J14" s="3">
+        <v>811681</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="M14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="N14" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K14" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="O14" s="6">
+        <v>21</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>8441146</v>
+      </c>
+      <c r="R14" t="s">
+        <v>262</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="C15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="7" t="s">
+      <c r="F15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J15" s="3">
+        <v>92840719</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="M15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="N15" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K15" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="O15" s="6">
+        <v>21</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>8392666</v>
+      </c>
+      <c r="R15" t="s">
+        <v>262</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F16" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G16" s="11" t="s">
+      <c r="F16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J16" s="3">
+        <v>27834401</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="H16" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="J16" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="O16" s="6">
+        <v>17</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>43277981</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="14" t="s">
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" s="6">
+        <v>9</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J17" s="3">
+        <v>94175962</v>
+      </c>
+      <c r="K17" t="s">
+        <v>269</v>
+      </c>
+      <c r="L17" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="M17" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F17" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="K17" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="N17" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="O17" s="6">
+        <v>22</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>29694749</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="14" t="s">
+      <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H18" s="6">
+        <v>11</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J18" s="3">
+        <v>122152275</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="M18" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="F18" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="J18" s="13" t="s">
-        <v>226</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="N18" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="O18" s="8">
+        <v>16</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>23690064</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="14" t="s">
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="6">
+        <v>18</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J19" s="3">
+        <v>58451088</v>
+      </c>
+      <c r="L19" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="M19" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="K19" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="N19" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="O19" s="6">
+        <v>5</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>163443671</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="14" t="s">
+      <c r="C20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H20" s="6">
+        <v>13</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J20" s="3">
+        <v>91350618</v>
+      </c>
+      <c r="L20" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="M20" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="N20" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="O20" s="6">
+        <v>10</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>87965473</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="14" t="s">
+      <c r="C21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="6">
+        <v>9</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J21" s="3">
+        <v>136670653</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="M21" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="K21" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="N21" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="O21" s="6">
+        <v>17</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>1422146</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="14" t="s">
+      <c r="C22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" s="6">
+        <v>11</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J22" s="3">
+        <v>111513451</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="M22" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="N22" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="O22" s="6">
+        <v>7</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>116796125</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="14" t="s">
+      <c r="C23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" s="6">
+        <v>21</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J23" s="3">
+        <v>25573983</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="M23" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="N23" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="O23" s="6">
+        <v>3</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>148742116</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="14" t="s">
+      <c r="C24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="6">
+        <v>17</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J24" s="3">
+        <v>48579904</v>
+      </c>
+      <c r="L24" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="M24" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F24" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="K24" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="N24" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="O24" s="6">
+        <v>7</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>27092993</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="14" t="s">
+      <c r="C25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H25" s="6">
+        <v>17</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J25" s="3">
+        <v>59841273</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="M25" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F25" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H25" s="14" t="s">
+      <c r="N25" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="O25" s="6">
+        <v>15</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>38488101</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="A26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="I25" s="12" t="s">
+      <c r="E26" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="F26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H26" s="6">
+        <v>8</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J26" s="3">
+        <v>143945206</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="N26" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="K25" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" t="s">
+      <c r="O26" s="6">
+        <v>14</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>105470216</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="A27" t="s">
         <v>211</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H26" s="14" t="s">
+      <c r="B27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="I26" s="12" t="s">
+      <c r="E27" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="F27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H27" s="6">
+        <v>2</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J27" s="3">
+        <v>219001648</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="K26" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" t="s">
+      <c r="O27" s="6">
+        <v>2</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>172595970</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="A28" t="s">
         <v>212</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H27" s="14" t="s">
+      <c r="B28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I27" s="12" t="s">
+      <c r="E28" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="J27" s="13" t="s">
+      <c r="F28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H28" s="6">
+        <v>19</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J28" s="3">
+        <v>53788748</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="K27" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" t="s">
+      <c r="O28" s="6">
+        <v>9</v>
+      </c>
+      <c r="P28" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>107306391</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19">
+      <c r="A29" t="s">
         <v>213</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H28" s="14" t="s">
+      <c r="B29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="I28" s="12" t="s">
+      <c r="E29" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="F29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H29" s="6">
+        <v>7</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J29" s="3">
+        <v>130877467</v>
+      </c>
+      <c r="K29" t="s">
+        <v>268</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="N29" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="K28" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" t="s">
+      <c r="O29" s="6">
+        <v>17</v>
+      </c>
+      <c r="P29" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>50184096</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19">
+      <c r="A30" t="s">
         <v>214</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H29" s="14" t="s">
+      <c r="B30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="E30" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="J29" s="13" t="s">
+      <c r="F30" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H30" s="6">
+        <v>3</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J30" s="3">
+        <v>37969413</v>
+      </c>
+      <c r="K30" t="s">
+        <v>267</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N30" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="K29" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" t="s">
+      <c r="O30" s="6">
+        <v>8</v>
+      </c>
+      <c r="P30" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>94880224</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19">
+      <c r="A31" t="s">
         <v>215</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H30" s="14" t="s">
+      <c r="B31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="I30" s="12" t="s">
+      <c r="E31" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="J30" s="13" t="s">
+      <c r="F31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H31" s="6">
+        <v>9</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J31" s="3">
+        <v>95086064</v>
+      </c>
+      <c r="K31" t="s">
+        <v>266</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="N31" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="K30" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" t="s">
+      <c r="O31" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="P31" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="R31" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" t="s">
         <v>216</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H31" s="14" t="s">
+      <c r="B32" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="E32" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="J31" s="13" t="s">
+      <c r="F32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H32" s="6">
+        <v>12</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J32" s="3">
+        <v>6964155</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N32" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="K31" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" t="s">
+      <c r="O32" s="6">
+        <v>11</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>18278670</v>
+      </c>
+      <c r="R32" t="s">
+        <v>262</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" t="s">
         <v>217</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G32" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H32" s="14" t="s">
+      <c r="B33" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="I32" s="12" t="s">
+      <c r="E33" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="J32" s="13" t="s">
+      <c r="F33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H33" s="6">
+        <v>9</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J33" s="3">
+        <v>95085505</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="N33" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="K32" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" t="s">
+      <c r="O33" s="6">
+        <v>2</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>38067603</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" t="s">
         <v>218</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H33" s="14" t="s">
+      <c r="B34" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="I33" s="12" t="s">
+      <c r="E34" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="J33" s="13" t="s">
+      <c r="F34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H34" s="6">
+        <v>1</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J34" s="3">
+        <v>65058442</v>
+      </c>
+      <c r="K34" t="s">
+        <v>265</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="N34" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="K33" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" t="s">
+      <c r="O34" s="6">
+        <v>7</v>
+      </c>
+      <c r="P34" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>148807372</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" t="s">
         <v>219</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H34" s="14" t="s">
+      <c r="B35" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="I34" s="12" t="s">
+      <c r="E35" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="F35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H35" s="6">
+        <v>6</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J35" s="3">
+        <v>52144401</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N35" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="K34" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
+      <c r="O35" s="6">
+        <v>3</v>
+      </c>
+      <c r="P35" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>120394214</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" t="s">
         <v>220</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G35" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H35" s="14" t="s">
+      <c r="B36" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="I35" s="12" t="s">
+      <c r="E36" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="J35" s="13" t="s">
+      <c r="F36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J36" s="3">
+        <v>45746180</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N36" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="K35" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" t="s">
+      <c r="O36" s="6">
+        <v>4</v>
+      </c>
+      <c r="P36" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>54738558</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19">
+      <c r="A37" t="s">
         <v>221</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H36" s="14" t="s">
+      <c r="B37" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="I36" s="12" t="s">
+      <c r="E37" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="J36" s="13" t="s">
+      <c r="F37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H37" s="6">
+        <v>22</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J37" s="3">
+        <v>46113691</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N37" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="K36" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11">
-      <c r="A37" t="s">
+      <c r="O37" s="6">
+        <v>1</v>
+      </c>
+      <c r="P37" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>26426242</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19">
+      <c r="A38" t="s">
         <v>222</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="I37" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="J37" s="13" t="s">
+      <c r="B38" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="K37" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" t="s">
+      <c r="C38" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H38" s="6">
+        <v>12</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J38" s="3">
+        <v>120293094</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="O38" s="6">
+        <v>15</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>67839940</v>
+      </c>
+      <c r="R38" t="s">
+        <v>260</v>
+      </c>
+      <c r="S38" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19">
+      <c r="A39" t="s">
         <v>223</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" s="17" t="s">
+      <c r="C39" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E39" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F38" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G38" s="15" t="s">
+      <c r="F39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H39" s="6">
+        <v>15</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J39" s="3">
+        <v>67839940</v>
+      </c>
+      <c r="K39" t="s">
+        <v>260</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M39" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="H38" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="I38" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="J38" s="16" t="s">
+      <c r="N39" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="K38" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" t="s">
-        <v>224</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="G39" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="I39" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="J39" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="K39" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="B41" s="3"/>
-      <c r="C41" s="4"/>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="B42" s="3"/>
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="B43" s="3"/>
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="B44" s="3"/>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="B45" s="3"/>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="B47" s="3"/>
-      <c r="C47" s="4"/>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="B48" s="3"/>
-      <c r="C48" s="4"/>
+      <c r="O39" s="6">
+        <v>17</v>
+      </c>
+      <c r="P39" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>43277981</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19">
+      <c r="B40" s="2"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:19">
+      <c r="B41" s="2"/>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:19">
+      <c r="B42" s="2"/>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:19">
+      <c r="B43" s="2"/>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:19">
+      <c r="B44" s="2"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:19">
+      <c r="B45" s="2"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:19">
+      <c r="B46" s="2"/>
+      <c r="C46" s="1"/>
+      <c r="K46" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19">
+      <c r="B47" s="2"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:19">
+      <c r="B48" s="2"/>
+      <c r="C48" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>